<commit_message>
Updating a comment and experimental results spreadsheet
</commit_message>
<xml_diff>
--- a/Experimental Results.xlsx
+++ b/Experimental Results.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Missed Annotations</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Limitations of Framework</t>
   </si>
@@ -47,13 +44,25 @@
     <t>Nullness</t>
   </si>
   <si>
-    <t>Explicit Checks Added</t>
-  </si>
-  <si>
     <t>Target Application</t>
   </si>
   <si>
     <t>SharpChecker</t>
+  </si>
+  <si>
+    <t>EventHub</t>
+  </si>
+  <si>
+    <t>Explicit Checks/Assertions Added</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Null reference exceptions were occurring when analyzing EventHub, and the class hierarchy issue was uncovered as a result of the method override checking (a little stretch).</t>
+  </si>
+  <si>
+    <t>There is an invocation which should be presenting a diagnostic, but is not.  It may be that that project is not being analzyed properly.</t>
   </si>
 </sst>
 </file>
@@ -89,8 +98,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,27 +383,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H4"/>
+  <dimension ref="A3:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="62.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -409,24 +421,66 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>4368</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
-        <v>7</v>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>268144</v>
+      </c>
+      <c r="E5">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4">
+      <c r="F5" t="s">
         <v>5</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed commented out code and updated comments.  Added an addtional annotation to the SharpChecker code to be enforced when the exercising the analysis on itself.
</commit_message>
<xml_diff>
--- a/Experimental Results.xlsx
+++ b/Experimental Results.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A3:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,13 +441,13 @@
         <v>4368</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="G4">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updating sandbox projects by adding nuget package.  This was necessary to expose the SharpChecker.Attributes  which are now in their own project.  Also, tweaked the nuspec to avoid a compiler warning.
</commit_message>
<xml_diff>
--- a/Experimental Results.xlsx
+++ b/Experimental Results.xlsx
@@ -62,7 +62,7 @@
     <t>Null reference exceptions were occurring when analyzing EventHub, and the class hierarchy issue was uncovered as a result of the method override checking (a little stretch).</t>
   </si>
   <si>
-    <t>There is an invocation which should be presenting a diagnostic, but is not.  It may be that that project is not being analzyed properly.</t>
+    <t>There is an invocation which should be presenting a diagnostic, but is not.  It may be that that project is not being analzyed properly.  I found that the Inteface needed to be annotated.  Also, async was not being properly analyzed.</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A3:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Adding a couple open source target applications used in validating SharpChecker
</commit_message>
<xml_diff>
--- a/Experimental Results.xlsx
+++ b/Experimental Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Limitations of Framework</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>There is an invocation which should be presenting a diagnostic, but is not.  It may be that that project is not being analzyed properly.  I found that the Inteface needed to be annotated.  Also, async was not being properly analyzed.</t>
+  </si>
+  <si>
+    <t>RijndaelEncryption</t>
+  </si>
+  <si>
+    <t>Encrypted</t>
   </si>
 </sst>
 </file>
@@ -383,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H5"/>
+  <dimension ref="A3:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,6 +485,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>